<commit_message>
Hardcoding the solcast api key as fallback
</commit_message>
<xml_diff>
--- a/Astro/Results_Production_Astro_xgb_15min.xlsx
+++ b/Astro/Results_Production_Astro_xgb_15min.xlsx
@@ -2427,7 +2427,7 @@
         <v>52</v>
       </c>
       <c r="C3">
-        <v>0.8070000000000001</v>
+        <v>0.821</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -2441,7 +2441,7 @@
         <v>53</v>
       </c>
       <c r="C4">
-        <v>0.759</v>
+        <v>0.787</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -2455,7 +2455,7 @@
         <v>54</v>
       </c>
       <c r="C5">
-        <v>0.666</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -2469,7 +2469,7 @@
         <v>55</v>
       </c>
       <c r="C6">
-        <v>0.759</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -2483,7 +2483,7 @@
         <v>56</v>
       </c>
       <c r="C7">
-        <v>0.793</v>
+        <v>0.716</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -2497,7 +2497,7 @@
         <v>57</v>
       </c>
       <c r="C8">
-        <v>0.781</v>
+        <v>0.785</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -2511,7 +2511,7 @@
         <v>58</v>
       </c>
       <c r="C9">
-        <v>0.773</v>
+        <v>0.779</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -2525,7 +2525,7 @@
         <v>59</v>
       </c>
       <c r="C10">
-        <v>0.762</v>
+        <v>0.753</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>

</xml_diff>